<commit_message>
oxidation-state (PC, PE, LPC, LPE), RT filter not for ox
- oxidation-state only for PC, PE, LPC and LPE
- no RT filtering for oxidized lipids
- pickBestMatchBySpectrumCoverage default off and only for ox-lipids
</commit_message>
<xml_diff>
--- a/installer/installFiles/exampleMassList/galactolipids_pos.xlsx
+++ b/installer/installFiles/exampleMassList/galactolipids_pos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="18660" yWindow="3672" windowWidth="22680" windowHeight="11076" activeTab="6"/>
+    <workbookView xWindow="18660" yWindow="3672" windowWidth="22680" windowHeight="11076" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="MGMG" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K463"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
     <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4290,8 +4290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K263"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11921,7 +11921,7 @@
   <dimension ref="A2:K463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11935,7 +11935,7 @@
     <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -20414,7 +20414,7 @@
   <dimension ref="A2:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -22996,7 +22996,7 @@
   <dimension ref="A2:L463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -23011,7 +23011,7 @@
     <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -32276,7 +32276,7 @@
   <dimension ref="A2:J263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -41412,8 +41412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44434,7 +44434,7 @@
   <dimension ref="A2:J263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -51277,7 +51277,7 @@
   <dimension ref="A2:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>